<commit_message>
Update mCODE r4 (ballot candidate)
</commit_message>
<xml_diff>
--- a/docs/mcode-r4/obf-CodedNonLaboratoryObservation.xlsx
+++ b/docs/mcode-r4/obf-CodedNonLaboratoryObservation.xlsx
@@ -395,7 +395,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest|ServiceRequest)
+    <t xml:space="preserve">Reference(MedicationRequest|ServiceRequest)
 </t>
   </si>
   <si>
@@ -565,7 +565,7 @@
     <t>Observation.subject</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/mcode/StructureDefinition/obf-Patient|Group|http://hl7.org/fhir/us/core/StructureDefinition/us-core-device|http://hl7.org/fhir/us/core/StructureDefinition/us-core-location)
+    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/mcode/StructureDefinition/obf-Patient|Group|Device|http://hl7.org/fhir/us/core/StructureDefinition/us-core-location)
 </t>
   </si>
   <si>
@@ -1090,7 +1090,7 @@
     <t>Observation.device</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/core/StructureDefinition/us-core-device)
+    <t xml:space="preserve">Reference(Device)
 </t>
   </si>
   <si>
@@ -1312,7 +1312,7 @@
     <t>Observation.derivedFrom</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference|Media|QuestionnaireResponse|http://hl7.org/fhir/us/mcode/StructureDefinition/obf-Observation)
+    <t xml:space="preserve">Reference(DocumentReference|Media|QuestionnaireResponse|http://hl7.org/fhir/us/mcode/StructureDefinition/obf-Observation)
 </t>
   </si>
   <si>

</xml_diff>